<commit_message>
-Fix default xLim/yLim -Read individual characteristics from XLS
</commit_message>
<xml_diff>
--- a/tests/data/CompiledDataSet.xlsx
+++ b/tests/data/CompiledDataSet.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A56DD2-474B-4D9F-AE6C-E7ED6C89E65F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84F8B64-48AE-4A7E-9F54-35ED7D77724F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1837" yWindow="1837" windowWidth="21600" windowHeight="11476" tabRatio="875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="59880" yWindow="2280" windowWidth="28800" windowHeight="15195" tabRatio="875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSheet_1" sheetId="1" r:id="rId1"/>
     <sheet name="MetaInfo" sheetId="48" r:id="rId2"/>
+    <sheet name="Stevens_2012_placebo" sheetId="49" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="73">
   <si>
     <t>Time [h]</t>
   </si>
@@ -397,6 +398,33 @@
   </si>
   <si>
     <t>MW</t>
+  </si>
+  <si>
+    <t>Time [min]</t>
+  </si>
+  <si>
+    <t>Fraction [%]</t>
+  </si>
+  <si>
+    <t>Error [%]</t>
+  </si>
+  <si>
+    <t>Placebo_total</t>
+  </si>
+  <si>
+    <t>Sita_total</t>
+  </si>
+  <si>
+    <t>Placebo_proximal</t>
+  </si>
+  <si>
+    <t>Sita_proximal</t>
+  </si>
+  <si>
+    <t>Placebo_distal</t>
+  </si>
+  <si>
+    <t>Sita_dist</t>
   </si>
 </sst>
 </file>
@@ -1284,29 +1312,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.59765625" customWidth="1"/>
+    <col min="1" max="1" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6328125" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1350,7 +1378,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -1388,7 +1416,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -1426,7 +1454,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1464,7 +1492,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -1502,7 +1530,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -1540,7 +1568,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -1578,7 +1606,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -1616,7 +1644,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -1654,7 +1682,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -1692,7 +1720,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -1730,7 +1758,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -1768,7 +1796,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -1819,16 +1847,16 @@
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.86328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.3984375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="22.59765625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="56.3984375" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="11.59765625" style="3"/>
+    <col min="1" max="1" width="12.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.36328125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="22.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.36328125" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="11.6328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C1" s="5" t="s">
         <v>14</v>
       </c>
@@ -1843,7 +1871,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C2" s="4" t="s">
         <v>17</v>
       </c>
@@ -1860,7 +1888,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C7" s="3" t="s">
         <v>22</v>
       </c>
@@ -1868,10 +1896,10 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C8" s="4"/>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C13" s="3" t="s">
         <v>24</v>
       </c>
@@ -1879,10 +1907,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C14" s="4"/>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C19" s="3" t="s">
         <v>27</v>
       </c>
@@ -1890,7 +1918,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C20" s="3" t="s">
         <v>28</v>
       </c>
@@ -1907,7 +1935,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
       <c r="E21" s="3" t="s">
         <v>31</v>
       </c>
@@ -1915,7 +1943,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
       <c r="E22" s="3" t="s">
         <v>36</v>
       </c>
@@ -1923,7 +1951,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.35">
       <c r="E23" s="3" t="s">
         <v>37</v>
       </c>
@@ -1931,7 +1959,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C24" s="3" t="s">
         <v>39</v>
       </c>
@@ -1942,7 +1970,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C25" s="3" t="s">
         <v>41</v>
       </c>
@@ -1953,7 +1981,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C26" s="3" t="s">
         <v>43</v>
       </c>
@@ -1967,7 +1995,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C27" s="3" t="s">
         <v>47</v>
       </c>
@@ -1987,13 +2015,1057 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8ECE4FC-F784-466F-BAAB-201D73E4B216}">
+  <dimension ref="A1:N78"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>100</v>
+      </c>
+      <c r="N2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J3">
+        <v>13.172268907563</v>
+      </c>
+      <c r="K3">
+        <v>93.75</v>
+      </c>
+      <c r="N3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J4">
+        <v>29.403361344537799</v>
+      </c>
+      <c r="K4">
+        <v>84.1666666666666</v>
+      </c>
+      <c r="N4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J5">
+        <v>44.647058823529399</v>
+      </c>
+      <c r="K5">
+        <v>72.5</v>
+      </c>
+      <c r="N5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J6">
+        <v>73.079831932773104</v>
+      </c>
+      <c r="K6">
+        <v>52.9166666666666</v>
+      </c>
+      <c r="N6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J7">
+        <v>88.273109243697405</v>
+      </c>
+      <c r="K7">
+        <v>46.25</v>
+      </c>
+      <c r="N7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J8">
+        <v>105.48319327730999</v>
+      </c>
+      <c r="K8">
+        <v>39.5833333333333</v>
+      </c>
+      <c r="N8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J9">
+        <v>118.66386554621801</v>
+      </c>
+      <c r="K9">
+        <v>32.5</v>
+      </c>
+      <c r="N9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J10">
+        <v>149.029411764705</v>
+      </c>
+      <c r="K10">
+        <v>21.25</v>
+      </c>
+      <c r="N10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J11">
+        <v>180.35294117647001</v>
+      </c>
+      <c r="K11">
+        <v>15</v>
+      </c>
+      <c r="N11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J12">
+        <v>210.65966386554601</v>
+      </c>
+      <c r="K12">
+        <v>9.5833333333333197</v>
+      </c>
+      <c r="N12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J13">
+        <v>240.94537815126</v>
+      </c>
+      <c r="K13">
+        <v>6.25</v>
+      </c>
+      <c r="N13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>100</v>
+      </c>
+      <c r="N14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J15">
+        <v>14.218487394957901</v>
+      </c>
+      <c r="K15">
+        <v>90</v>
+      </c>
+      <c r="N15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J16">
+        <v>27.403361344537799</v>
+      </c>
+      <c r="K16">
+        <v>82.5</v>
+      </c>
+      <c r="N16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J17">
+        <v>43.634453781512597</v>
+      </c>
+      <c r="K17">
+        <v>72.9166666666666</v>
+      </c>
+      <c r="N17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J18">
+        <v>57.8403361344537</v>
+      </c>
+      <c r="K18">
+        <v>64.1666666666666</v>
+      </c>
+      <c r="N18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J19">
+        <v>74.067226890756302</v>
+      </c>
+      <c r="K19">
+        <v>55</v>
+      </c>
+      <c r="N19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J20">
+        <v>89.260504201680604</v>
+      </c>
+      <c r="K20">
+        <v>48.3333333333333</v>
+      </c>
+      <c r="N20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J21">
+        <v>105.462184873949</v>
+      </c>
+      <c r="K21">
+        <v>41.6666666666666</v>
+      </c>
+      <c r="N21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J22">
+        <v>119.642857142857</v>
+      </c>
+      <c r="K22">
+        <v>35.4166666666666</v>
+      </c>
+      <c r="N22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J23">
+        <v>150.004201680672</v>
+      </c>
+      <c r="K23">
+        <v>24.5833333333333</v>
+      </c>
+      <c r="N23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J24">
+        <v>179.31932773109199</v>
+      </c>
+      <c r="K24">
+        <v>17.5</v>
+      </c>
+      <c r="N24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J25">
+        <v>209.62605042016801</v>
+      </c>
+      <c r="K25">
+        <v>12.0833333333333</v>
+      </c>
+      <c r="N25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J26">
+        <v>240.915966386554</v>
+      </c>
+      <c r="K26">
+        <v>9.1666666666666803</v>
+      </c>
+      <c r="N26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J27">
+        <v>0.967598097502957</v>
+      </c>
+      <c r="K27">
+        <v>74.482758620689594</v>
+      </c>
+      <c r="L27">
+        <v>4.827586206896612</v>
+      </c>
+      <c r="N27" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J28">
+        <v>16.306480380499401</v>
+      </c>
+      <c r="K28">
+        <v>60.689655172413801</v>
+      </c>
+      <c r="L28">
+        <v>2.0689655172413026</v>
+      </c>
+      <c r="N28" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J29">
+        <v>30.659928656361402</v>
+      </c>
+      <c r="K29">
+        <v>50.689655172413801</v>
+      </c>
+      <c r="L29">
+        <v>3.1034482758620001</v>
+      </c>
+      <c r="N29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J30">
+        <v>45.026753864447002</v>
+      </c>
+      <c r="K30">
+        <v>41.724137931034399</v>
+      </c>
+      <c r="L30">
+        <v>1.7241379310344982</v>
+      </c>
+      <c r="N30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J31">
+        <v>61.475921521997499</v>
+      </c>
+      <c r="K31">
+        <v>33.793103448275801</v>
+      </c>
+      <c r="L31">
+        <v>2.7586206896551957</v>
+      </c>
+      <c r="N31" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J32">
+        <v>74.839476813317404</v>
+      </c>
+      <c r="K32">
+        <v>27.241379310344801</v>
+      </c>
+      <c r="L32">
+        <v>2.4137931034482989</v>
+      </c>
+      <c r="N32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J33">
+        <v>90.303210463733507</v>
+      </c>
+      <c r="K33">
+        <v>23.103448275862</v>
+      </c>
+      <c r="L33">
+        <v>2.4137931034482989</v>
+      </c>
+      <c r="N33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J34">
+        <v>105.76248513674101</v>
+      </c>
+      <c r="K34">
+        <v>18.620689655172399</v>
+      </c>
+      <c r="L34">
+        <v>2.413793103448203</v>
+      </c>
+      <c r="N34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J35">
+        <v>121.23513674197299</v>
+      </c>
+      <c r="K35">
+        <v>15.1724137931034</v>
+      </c>
+      <c r="L35">
+        <v>2.758620689655201</v>
+      </c>
+      <c r="N35" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J36">
+        <v>150.133769322235</v>
+      </c>
+      <c r="K36">
+        <v>10</v>
+      </c>
+      <c r="L36">
+        <v>2.7586206896550998</v>
+      </c>
+      <c r="N36" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J37">
+        <v>182.16260404280601</v>
+      </c>
+      <c r="K37">
+        <v>6.8965517241379297</v>
+      </c>
+      <c r="L37">
+        <v>2.068965517241371</v>
+      </c>
+      <c r="N37" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J38">
+        <v>211.09690844233</v>
+      </c>
+      <c r="K38">
+        <v>4.4827586206896601</v>
+      </c>
+      <c r="N38" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J39">
+        <v>242.11355529131899</v>
+      </c>
+      <c r="K39">
+        <v>3.1034482758620601</v>
+      </c>
+      <c r="N39" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J40">
+        <v>0.967598097502957</v>
+      </c>
+      <c r="K40">
+        <v>74.482758620689594</v>
+      </c>
+      <c r="L40">
+        <v>4.827586206896612</v>
+      </c>
+      <c r="N40" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J41">
+        <v>16.306480380499401</v>
+      </c>
+      <c r="K41">
+        <v>60.689655172413801</v>
+      </c>
+      <c r="L41">
+        <v>2.0689655172413026</v>
+      </c>
+      <c r="N41" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J42">
+        <v>30.659928656361402</v>
+      </c>
+      <c r="K42">
+        <v>50.689655172413801</v>
+      </c>
+      <c r="L42">
+        <v>3.1034482758620001</v>
+      </c>
+      <c r="N42" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J43">
+        <v>45.026753864447002</v>
+      </c>
+      <c r="K43">
+        <v>41.724137931034399</v>
+      </c>
+      <c r="L43">
+        <v>1.7241379310344982</v>
+      </c>
+      <c r="N43" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J44">
+        <v>61.475921521997499</v>
+      </c>
+      <c r="K44">
+        <v>33.793103448275801</v>
+      </c>
+      <c r="L44">
+        <v>2.7586206896551957</v>
+      </c>
+      <c r="N44" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J45">
+        <v>74.839476813317404</v>
+      </c>
+      <c r="K45">
+        <v>27.241379310344801</v>
+      </c>
+      <c r="L45">
+        <v>2.4137931034482989</v>
+      </c>
+      <c r="N45" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J46">
+        <v>90.303210463733507</v>
+      </c>
+      <c r="K46">
+        <v>23.103448275862</v>
+      </c>
+      <c r="L46">
+        <v>2.4137931034482989</v>
+      </c>
+      <c r="N46" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J47">
+        <v>105.76248513674101</v>
+      </c>
+      <c r="K47">
+        <v>18.620689655172399</v>
+      </c>
+      <c r="L47">
+        <v>2.413793103448203</v>
+      </c>
+      <c r="N47" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J48">
+        <v>121.23513674197299</v>
+      </c>
+      <c r="K48">
+        <v>15.1724137931034</v>
+      </c>
+      <c r="L48">
+        <v>2.758620689655201</v>
+      </c>
+      <c r="N48" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J49">
+        <v>150.133769322235</v>
+      </c>
+      <c r="K49">
+        <v>10</v>
+      </c>
+      <c r="L49">
+        <v>2.7586206896550998</v>
+      </c>
+      <c r="N49" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J50">
+        <v>182.16260404280601</v>
+      </c>
+      <c r="K50">
+        <v>6.8965517241379297</v>
+      </c>
+      <c r="L50">
+        <v>2.068965517241371</v>
+      </c>
+      <c r="N50" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J51">
+        <v>211.09690844233</v>
+      </c>
+      <c r="K51">
+        <v>4.4827586206896601</v>
+      </c>
+      <c r="N51" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J52">
+        <v>242.11355529131899</v>
+      </c>
+      <c r="K52">
+        <v>3.1034482758620601</v>
+      </c>
+      <c r="N52" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J53">
+        <v>0</v>
+      </c>
+      <c r="K53">
+        <v>25.579399141630901</v>
+      </c>
+      <c r="L53">
+        <v>2.7467811158797986</v>
+      </c>
+      <c r="N53" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="54" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J54">
+        <v>14.482758620689699</v>
+      </c>
+      <c r="K54">
+        <v>32.446351931330398</v>
+      </c>
+      <c r="L54">
+        <v>2.9184549356223002</v>
+      </c>
+      <c r="N54" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="55" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J55">
+        <v>28.965517241379299</v>
+      </c>
+      <c r="K55">
+        <v>32.103004291845401</v>
+      </c>
+      <c r="L55">
+        <v>2.7467811158798021</v>
+      </c>
+      <c r="N55" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="56" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J56">
+        <v>45.517241379310398</v>
+      </c>
+      <c r="K56">
+        <v>30.2145922746781</v>
+      </c>
+      <c r="L56">
+        <v>2.4034334763949019</v>
+      </c>
+      <c r="N56" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="57" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J57">
+        <v>58.965517241379402</v>
+      </c>
+      <c r="K57">
+        <v>29.0128755364806</v>
+      </c>
+      <c r="L57">
+        <v>2.2317596566523008</v>
+      </c>
+      <c r="N57" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="58" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J58">
+        <v>74.482758620689694</v>
+      </c>
+      <c r="K58">
+        <v>25.7510729613733</v>
+      </c>
+      <c r="L58">
+        <v>2.0600858369097992</v>
+      </c>
+      <c r="N58" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="59" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J59">
+        <v>88.965517241379402</v>
+      </c>
+      <c r="K59">
+        <v>22.317596566523601</v>
+      </c>
+      <c r="L59">
+        <v>1.7167381974249025</v>
+      </c>
+      <c r="N59" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="60" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J60">
+        <v>104.482758620689</v>
+      </c>
+      <c r="K60">
+        <v>19.399141630901202</v>
+      </c>
+      <c r="L60">
+        <v>1.716738197424803</v>
+      </c>
+      <c r="N60" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="61" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J61">
+        <v>120</v>
+      </c>
+      <c r="K61">
+        <v>16.480686695278902</v>
+      </c>
+      <c r="L61">
+        <v>1.5450643776824009</v>
+      </c>
+      <c r="N61" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="62" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J62">
+        <v>150</v>
+      </c>
+      <c r="K62">
+        <v>11.158798283261801</v>
+      </c>
+      <c r="L62">
+        <v>1.2017167381974208</v>
+      </c>
+      <c r="N62" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="63" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J63">
+        <v>180</v>
+      </c>
+      <c r="K63">
+        <v>8.2403433476394792</v>
+      </c>
+      <c r="L63">
+        <v>0.85836909871243883</v>
+      </c>
+      <c r="N63" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="64" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J64">
+        <v>211.03448275861999</v>
+      </c>
+      <c r="K64">
+        <v>5.3218884120171701</v>
+      </c>
+      <c r="L64">
+        <v>1.0300429184549404</v>
+      </c>
+      <c r="N64" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="65" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J65">
+        <v>238.96551724137899</v>
+      </c>
+      <c r="K65">
+        <v>4.1201716738197396</v>
+      </c>
+      <c r="L65">
+        <v>0.51502145922746978</v>
+      </c>
+      <c r="N65" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="66" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J66">
+        <v>0</v>
+      </c>
+      <c r="K66">
+        <v>24.206008583690899</v>
+      </c>
+      <c r="L66">
+        <v>2.7467811158797986</v>
+      </c>
+      <c r="N66" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="67" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J67">
+        <v>14.482758620689699</v>
+      </c>
+      <c r="K67">
+        <v>31.244635193133</v>
+      </c>
+      <c r="L67">
+        <v>2.5751072961373005</v>
+      </c>
+      <c r="N67" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="68" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J68">
+        <v>26.8965517241379</v>
+      </c>
+      <c r="K68">
+        <v>32.274678111587903</v>
+      </c>
+      <c r="L68">
+        <v>2.9184549356223037</v>
+      </c>
+      <c r="N68" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="69" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J69">
+        <v>44.482758620689701</v>
+      </c>
+      <c r="K69">
+        <v>31.244635193133</v>
+      </c>
+      <c r="L69">
+        <v>2.4034334763949019</v>
+      </c>
+      <c r="N69" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="70" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J70">
+        <v>61.034482758620797</v>
+      </c>
+      <c r="K70">
+        <v>29.356223175965599</v>
+      </c>
+      <c r="L70">
+        <v>2.7467811158798021</v>
+      </c>
+      <c r="N70" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="71" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J71">
+        <v>74.482758620689694</v>
+      </c>
+      <c r="K71">
+        <v>27.9828326180257</v>
+      </c>
+      <c r="L71">
+        <v>2.2317596566524003</v>
+      </c>
+      <c r="N71" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="72" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J72">
+        <v>90.000000000000099</v>
+      </c>
+      <c r="K72">
+        <v>25.0643776824034</v>
+      </c>
+      <c r="L72">
+        <v>2.7467811158797986</v>
+      </c>
+      <c r="N72" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="73" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J73">
+        <v>104.482758620689</v>
+      </c>
+      <c r="K73">
+        <v>21.8025751072961</v>
+      </c>
+      <c r="L73">
+        <v>2.7467811158797986</v>
+      </c>
+      <c r="N73" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J74">
+        <v>118.965517241379</v>
+      </c>
+      <c r="K74">
+        <v>19.2274678111588</v>
+      </c>
+      <c r="L74">
+        <v>2.4034334763947989</v>
+      </c>
+      <c r="N74" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J75">
+        <v>148.96551724137899</v>
+      </c>
+      <c r="K75">
+        <v>13.5622317596566</v>
+      </c>
+      <c r="L75">
+        <v>2.2317596566524003</v>
+      </c>
+      <c r="N75" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="76" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J76">
+        <v>180</v>
+      </c>
+      <c r="K76">
+        <v>9.6137339055793998</v>
+      </c>
+      <c r="L76">
+        <v>2.4034334763948006</v>
+      </c>
+      <c r="N76" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="77" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J77">
+        <v>208.96551724137899</v>
+      </c>
+      <c r="K77">
+        <v>6.5236051502145997</v>
+      </c>
+      <c r="L77">
+        <v>1.8884120171673704</v>
+      </c>
+      <c r="N77" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="78" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J78">
+        <v>240</v>
+      </c>
+      <c r="K78">
+        <v>5.1502145922746703</v>
+      </c>
+      <c r="L78">
+        <v>1.8884120171673899</v>
+      </c>
+      <c r="N78" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2002,7 +3074,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b6960b7ce0e258e5d224c1a71edff679">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e7db7ba54f101f424e932c64edcbdaa0" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -2219,23 +3291,13 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07F0F837-F7F5-4F1A-B3BF-0AF8EF39D57E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68DDEE09-40A7-45D2-BB9E-2F87B709C6D9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -2243,7 +3305,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCE8CCCB-E073-4D73-9695-C91416D097D2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2260,4 +3322,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07F0F837-F7F5-4F1A-B3BF-0AF8EF39D57E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Reading parameters from xls now allows extra columns to be present.
</commit_message>
<xml_diff>
--- a/tests/data/CompiledDataSet.xlsx
+++ b/tests/data/CompiledDataSet.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB7AD7DE-CF5F-4092-AE2B-7C958088101C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E4F2BB-5A0B-4B6D-849F-7AD76D999ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1988" yWindow="2520" windowWidth="21600" windowHeight="11535" tabRatio="875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-113" yWindow="-113" windowWidth="29026" windowHeight="15825" tabRatio="875" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSheet_1" sheetId="1" r:id="rId1"/>
     <sheet name="MetaInfo" sheetId="48" r:id="rId2"/>
     <sheet name="Stevens_2012_placebo" sheetId="49" r:id="rId3"/>
+    <sheet name="WrongSheet" sheetId="50" r:id="rId4"/>
+    <sheet name="CorrectSheet_additionalCols" sheetId="51" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="74">
   <si>
     <t>Time [h]</t>
   </si>
@@ -2022,8 +2024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA0E8DDA-F3F4-4710-A6B6-93A80B4A8C1A}">
   <dimension ref="A1:N78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection sqref="A1:N78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3068,7 +3070,1131 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CCB5B98-2408-40BA-99F9-228ECCEE7326}">
+  <dimension ref="A1:N1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:N1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C19160-8B30-4C70-A987-7318B15033AF}">
+  <dimension ref="A1:Q78"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:N78"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>100</v>
+      </c>
+      <c r="N2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="J3">
+        <v>13.172268907563</v>
+      </c>
+      <c r="K3">
+        <v>93.75</v>
+      </c>
+      <c r="N3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="J4">
+        <v>29.403361344537799</v>
+      </c>
+      <c r="K4">
+        <v>84.1666666666666</v>
+      </c>
+      <c r="N4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="J5">
+        <v>44.647058823529399</v>
+      </c>
+      <c r="K5">
+        <v>72.5</v>
+      </c>
+      <c r="N5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="J6">
+        <v>73.079831932773104</v>
+      </c>
+      <c r="K6">
+        <v>52.9166666666666</v>
+      </c>
+      <c r="N6" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="J7">
+        <v>88.273109243697405</v>
+      </c>
+      <c r="K7">
+        <v>46.25</v>
+      </c>
+      <c r="N7" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="J8">
+        <v>105.48319327730999</v>
+      </c>
+      <c r="K8">
+        <v>39.5833333333333</v>
+      </c>
+      <c r="N8" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="J9">
+        <v>118.66386554621801</v>
+      </c>
+      <c r="K9">
+        <v>32.5</v>
+      </c>
+      <c r="N9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="J10">
+        <v>149.029411764705</v>
+      </c>
+      <c r="K10">
+        <v>21.25</v>
+      </c>
+      <c r="N10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="J11">
+        <v>180.35294117647001</v>
+      </c>
+      <c r="K11">
+        <v>15</v>
+      </c>
+      <c r="N11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="J12">
+        <v>210.65966386554601</v>
+      </c>
+      <c r="K12">
+        <v>9.5833333333333197</v>
+      </c>
+      <c r="N12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="J13">
+        <v>240.94537815126</v>
+      </c>
+      <c r="K13">
+        <v>6.25</v>
+      </c>
+      <c r="N13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>100</v>
+      </c>
+      <c r="N14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="J15">
+        <v>14.218487394957901</v>
+      </c>
+      <c r="K15">
+        <v>90</v>
+      </c>
+      <c r="N15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="J16">
+        <v>27.403361344537799</v>
+      </c>
+      <c r="K16">
+        <v>82.5</v>
+      </c>
+      <c r="N16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J17">
+        <v>43.634453781512597</v>
+      </c>
+      <c r="K17">
+        <v>72.9166666666666</v>
+      </c>
+      <c r="N17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J18">
+        <v>57.8403361344537</v>
+      </c>
+      <c r="K18">
+        <v>64.1666666666666</v>
+      </c>
+      <c r="N18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J19">
+        <v>74.067226890756302</v>
+      </c>
+      <c r="K19">
+        <v>55</v>
+      </c>
+      <c r="N19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J20">
+        <v>89.260504201680604</v>
+      </c>
+      <c r="K20">
+        <v>48.3333333333333</v>
+      </c>
+      <c r="N20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J21">
+        <v>105.462184873949</v>
+      </c>
+      <c r="K21">
+        <v>41.6666666666666</v>
+      </c>
+      <c r="N21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J22">
+        <v>119.642857142857</v>
+      </c>
+      <c r="K22">
+        <v>35.4166666666666</v>
+      </c>
+      <c r="N22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J23">
+        <v>150.004201680672</v>
+      </c>
+      <c r="K23">
+        <v>24.5833333333333</v>
+      </c>
+      <c r="N23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J24">
+        <v>179.31932773109199</v>
+      </c>
+      <c r="K24">
+        <v>17.5</v>
+      </c>
+      <c r="N24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J25">
+        <v>209.62605042016801</v>
+      </c>
+      <c r="K25">
+        <v>12.0833333333333</v>
+      </c>
+      <c r="N25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J26">
+        <v>240.915966386554</v>
+      </c>
+      <c r="K26">
+        <v>9.1666666666666803</v>
+      </c>
+      <c r="N26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J27">
+        <v>0.967598097502957</v>
+      </c>
+      <c r="K27">
+        <v>74.482758620689594</v>
+      </c>
+      <c r="L27">
+        <v>4.827586206896612</v>
+      </c>
+      <c r="N27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J28">
+        <v>16.306480380499401</v>
+      </c>
+      <c r="K28">
+        <v>60.689655172413801</v>
+      </c>
+      <c r="L28">
+        <v>2.0689655172413026</v>
+      </c>
+      <c r="N28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J29">
+        <v>30.659928656361402</v>
+      </c>
+      <c r="K29">
+        <v>50.689655172413801</v>
+      </c>
+      <c r="L29">
+        <v>3.1034482758620001</v>
+      </c>
+      <c r="N29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J30">
+        <v>45.026753864447002</v>
+      </c>
+      <c r="K30">
+        <v>41.724137931034399</v>
+      </c>
+      <c r="L30">
+        <v>1.7241379310344982</v>
+      </c>
+      <c r="N30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J31">
+        <v>61.475921521997499</v>
+      </c>
+      <c r="K31">
+        <v>33.793103448275801</v>
+      </c>
+      <c r="L31">
+        <v>2.7586206896551957</v>
+      </c>
+      <c r="N31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J32">
+        <v>74.839476813317404</v>
+      </c>
+      <c r="K32">
+        <v>27.241379310344801</v>
+      </c>
+      <c r="L32">
+        <v>2.4137931034482989</v>
+      </c>
+      <c r="N32" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J33">
+        <v>90.303210463733507</v>
+      </c>
+      <c r="K33">
+        <v>23.103448275862</v>
+      </c>
+      <c r="L33">
+        <v>2.4137931034482989</v>
+      </c>
+      <c r="N33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J34">
+        <v>105.76248513674101</v>
+      </c>
+      <c r="K34">
+        <v>18.620689655172399</v>
+      </c>
+      <c r="L34">
+        <v>2.413793103448203</v>
+      </c>
+      <c r="N34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J35">
+        <v>121.23513674197299</v>
+      </c>
+      <c r="K35">
+        <v>15.1724137931034</v>
+      </c>
+      <c r="L35">
+        <v>2.758620689655201</v>
+      </c>
+      <c r="N35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J36">
+        <v>150.133769322235</v>
+      </c>
+      <c r="K36">
+        <v>10</v>
+      </c>
+      <c r="L36">
+        <v>2.7586206896550998</v>
+      </c>
+      <c r="N36" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J37">
+        <v>182.16260404280601</v>
+      </c>
+      <c r="K37">
+        <v>6.8965517241379297</v>
+      </c>
+      <c r="L37">
+        <v>2.068965517241371</v>
+      </c>
+      <c r="N37" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J38">
+        <v>211.09690844233</v>
+      </c>
+      <c r="K38">
+        <v>4.4827586206896601</v>
+      </c>
+      <c r="N38" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J39">
+        <v>242.11355529131899</v>
+      </c>
+      <c r="K39">
+        <v>3.1034482758620601</v>
+      </c>
+      <c r="N39" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J40">
+        <v>0.967598097502957</v>
+      </c>
+      <c r="K40">
+        <v>74.482758620689594</v>
+      </c>
+      <c r="L40">
+        <v>4.827586206896612</v>
+      </c>
+      <c r="N40" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J41">
+        <v>16.306480380499401</v>
+      </c>
+      <c r="K41">
+        <v>60.689655172413801</v>
+      </c>
+      <c r="L41">
+        <v>2.0689655172413026</v>
+      </c>
+      <c r="N41" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J42">
+        <v>30.659928656361402</v>
+      </c>
+      <c r="K42">
+        <v>50.689655172413801</v>
+      </c>
+      <c r="L42">
+        <v>3.1034482758620001</v>
+      </c>
+      <c r="N42" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J43">
+        <v>45.026753864447002</v>
+      </c>
+      <c r="K43">
+        <v>41.724137931034399</v>
+      </c>
+      <c r="L43">
+        <v>1.7241379310344982</v>
+      </c>
+      <c r="N43" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J44">
+        <v>61.475921521997499</v>
+      </c>
+      <c r="K44">
+        <v>33.793103448275801</v>
+      </c>
+      <c r="L44">
+        <v>2.7586206896551957</v>
+      </c>
+      <c r="N44" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J45">
+        <v>74.839476813317404</v>
+      </c>
+      <c r="K45">
+        <v>27.241379310344801</v>
+      </c>
+      <c r="L45">
+        <v>2.4137931034482989</v>
+      </c>
+      <c r="N45" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J46">
+        <v>90.303210463733507</v>
+      </c>
+      <c r="K46">
+        <v>23.103448275862</v>
+      </c>
+      <c r="L46">
+        <v>2.4137931034482989</v>
+      </c>
+      <c r="N46" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="47" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J47">
+        <v>105.76248513674101</v>
+      </c>
+      <c r="K47">
+        <v>18.620689655172399</v>
+      </c>
+      <c r="L47">
+        <v>2.413793103448203</v>
+      </c>
+      <c r="N47" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J48">
+        <v>121.23513674197299</v>
+      </c>
+      <c r="K48">
+        <v>15.1724137931034</v>
+      </c>
+      <c r="L48">
+        <v>2.758620689655201</v>
+      </c>
+      <c r="N48" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="49" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J49">
+        <v>150.133769322235</v>
+      </c>
+      <c r="K49">
+        <v>10</v>
+      </c>
+      <c r="L49">
+        <v>2.7586206896550998</v>
+      </c>
+      <c r="N49" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="50" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J50">
+        <v>182.16260404280601</v>
+      </c>
+      <c r="K50">
+        <v>6.8965517241379297</v>
+      </c>
+      <c r="L50">
+        <v>2.068965517241371</v>
+      </c>
+      <c r="N50" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="51" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J51">
+        <v>211.09690844233</v>
+      </c>
+      <c r="K51">
+        <v>4.4827586206896601</v>
+      </c>
+      <c r="N51" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="52" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J52">
+        <v>242.11355529131899</v>
+      </c>
+      <c r="K52">
+        <v>3.1034482758620601</v>
+      </c>
+      <c r="N52" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="53" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J53">
+        <v>0</v>
+      </c>
+      <c r="K53">
+        <v>25.579399141630901</v>
+      </c>
+      <c r="L53">
+        <v>2.7467811158797986</v>
+      </c>
+      <c r="N53" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="54" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J54">
+        <v>14.482758620689699</v>
+      </c>
+      <c r="K54">
+        <v>32.446351931330398</v>
+      </c>
+      <c r="L54">
+        <v>2.9184549356223002</v>
+      </c>
+      <c r="N54" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J55">
+        <v>28.965517241379299</v>
+      </c>
+      <c r="K55">
+        <v>32.103004291845401</v>
+      </c>
+      <c r="L55">
+        <v>2.7467811158798021</v>
+      </c>
+      <c r="N55" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="56" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J56">
+        <v>45.517241379310398</v>
+      </c>
+      <c r="K56">
+        <v>30.2145922746781</v>
+      </c>
+      <c r="L56">
+        <v>2.4034334763949019</v>
+      </c>
+      <c r="N56" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="57" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J57">
+        <v>58.965517241379402</v>
+      </c>
+      <c r="K57">
+        <v>29.0128755364806</v>
+      </c>
+      <c r="L57">
+        <v>2.2317596566523008</v>
+      </c>
+      <c r="N57" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="58" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J58">
+        <v>74.482758620689694</v>
+      </c>
+      <c r="K58">
+        <v>25.7510729613733</v>
+      </c>
+      <c r="L58">
+        <v>2.0600858369097992</v>
+      </c>
+      <c r="N58" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="59" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J59">
+        <v>88.965517241379402</v>
+      </c>
+      <c r="K59">
+        <v>22.317596566523601</v>
+      </c>
+      <c r="L59">
+        <v>1.7167381974249025</v>
+      </c>
+      <c r="N59" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="60" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J60">
+        <v>104.482758620689</v>
+      </c>
+      <c r="K60">
+        <v>19.399141630901202</v>
+      </c>
+      <c r="L60">
+        <v>1.716738197424803</v>
+      </c>
+      <c r="N60" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="61" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J61">
+        <v>120</v>
+      </c>
+      <c r="K61">
+        <v>16.480686695278902</v>
+      </c>
+      <c r="L61">
+        <v>1.5450643776824009</v>
+      </c>
+      <c r="N61" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="62" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J62">
+        <v>150</v>
+      </c>
+      <c r="K62">
+        <v>11.158798283261801</v>
+      </c>
+      <c r="L62">
+        <v>1.2017167381974208</v>
+      </c>
+      <c r="N62" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="63" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J63">
+        <v>180</v>
+      </c>
+      <c r="K63">
+        <v>8.2403433476394792</v>
+      </c>
+      <c r="L63">
+        <v>0.85836909871243883</v>
+      </c>
+      <c r="N63" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="64" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J64">
+        <v>211.03448275861999</v>
+      </c>
+      <c r="K64">
+        <v>5.3218884120171701</v>
+      </c>
+      <c r="L64">
+        <v>1.0300429184549404</v>
+      </c>
+      <c r="N64" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="65" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J65">
+        <v>238.96551724137899</v>
+      </c>
+      <c r="K65">
+        <v>4.1201716738197396</v>
+      </c>
+      <c r="L65">
+        <v>0.51502145922746978</v>
+      </c>
+      <c r="N65" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="66" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J66">
+        <v>0</v>
+      </c>
+      <c r="K66">
+        <v>24.206008583690899</v>
+      </c>
+      <c r="L66">
+        <v>2.7467811158797986</v>
+      </c>
+      <c r="N66" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="67" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J67">
+        <v>14.482758620689699</v>
+      </c>
+      <c r="K67">
+        <v>31.244635193133</v>
+      </c>
+      <c r="L67">
+        <v>2.5751072961373005</v>
+      </c>
+      <c r="N67" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="68" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J68">
+        <v>26.8965517241379</v>
+      </c>
+      <c r="K68">
+        <v>32.274678111587903</v>
+      </c>
+      <c r="L68">
+        <v>2.9184549356223037</v>
+      </c>
+      <c r="N68" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="69" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J69">
+        <v>44.482758620689701</v>
+      </c>
+      <c r="K69">
+        <v>31.244635193133</v>
+      </c>
+      <c r="L69">
+        <v>2.4034334763949019</v>
+      </c>
+      <c r="N69" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="70" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J70">
+        <v>61.034482758620797</v>
+      </c>
+      <c r="K70">
+        <v>29.356223175965599</v>
+      </c>
+      <c r="L70">
+        <v>2.7467811158798021</v>
+      </c>
+      <c r="N70" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="71" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J71">
+        <v>74.482758620689694</v>
+      </c>
+      <c r="K71">
+        <v>27.9828326180257</v>
+      </c>
+      <c r="L71">
+        <v>2.2317596566524003</v>
+      </c>
+      <c r="N71" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="72" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J72">
+        <v>90.000000000000099</v>
+      </c>
+      <c r="K72">
+        <v>25.0643776824034</v>
+      </c>
+      <c r="L72">
+        <v>2.7467811158797986</v>
+      </c>
+      <c r="N72" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="73" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J73">
+        <v>104.482758620689</v>
+      </c>
+      <c r="K73">
+        <v>21.8025751072961</v>
+      </c>
+      <c r="L73">
+        <v>2.7467811158797986</v>
+      </c>
+      <c r="N73" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J74">
+        <v>118.965517241379</v>
+      </c>
+      <c r="K74">
+        <v>19.2274678111588</v>
+      </c>
+      <c r="L74">
+        <v>2.4034334763947989</v>
+      </c>
+      <c r="N74" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J75">
+        <v>148.96551724137899</v>
+      </c>
+      <c r="K75">
+        <v>13.5622317596566</v>
+      </c>
+      <c r="L75">
+        <v>2.2317596566524003</v>
+      </c>
+      <c r="N75" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J76">
+        <v>180</v>
+      </c>
+      <c r="K76">
+        <v>9.6137339055793998</v>
+      </c>
+      <c r="L76">
+        <v>2.4034334763948006</v>
+      </c>
+      <c r="N76" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="77" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J77">
+        <v>208.96551724137899</v>
+      </c>
+      <c r="K77">
+        <v>6.5236051502145997</v>
+      </c>
+      <c r="L77">
+        <v>1.8884120171673704</v>
+      </c>
+      <c r="N77" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="78" spans="10:14" x14ac:dyDescent="0.45">
+      <c r="J78">
+        <v>240</v>
+      </c>
+      <c r="K78">
+        <v>5.1502145922746703</v>
+      </c>
+      <c r="L78">
+        <v>1.8884120171673899</v>
+      </c>
+      <c r="N78" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b6960b7ce0e258e5d224c1a71edff679">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e7db7ba54f101f424e932c64edcbdaa0" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -3285,7 +4411,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -3294,13 +4420,23 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07F0F837-F7F5-4F1A-B3BF-0AF8EF39D57E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCE8CCCB-E073-4D73-9695-C91416D097D2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3319,26 +4455,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68DDEE09-40A7-45D2-BB9E-2F87B709C6D9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07F0F837-F7F5-4F1A-B3BF-0AF8EF39D57E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>